<commit_message>
Update template metadata for new database
</commit_message>
<xml_diff>
--- a/templates/2EXT01_RNA.xlsx
+++ b/templates/2EXT01_RNA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4585D2-C512-4B14-9AB4-4C0CA2DA6936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E9EB81-5318-4B8B-8DD1-F47938B6FE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT01_RNA" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,14 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={B2C9D632-6E8E-4E4D-B849-13347E0E2396}</author>
+    <author>tc={A496038F-2B69-4D66-8B22-6FE82F201B1B}</author>
+    <author>tc={4FEB2A0D-0D69-4C74-90F9-B60ACAD3FC0E}</author>
+    <author>tc={B81587F8-24F1-4441-B5CF-797CFF5344EB}</author>
+    <author>tc={AB998CBF-C99C-4803-A8E4-15BF70F85D88}</author>
+    <author>tc={702BED30-27FB-4E09-A198-242406CDD04B}</author>
+    <author>tc={6883E21B-C50F-46D5-8D5C-2A49F4678F53}</author>
+    <author>tc={A49430D7-EB67-44F6-A021-4724976004EE}</author>
+    <author>tc={E3637547-CF61-40AD-92E9-13EEE0777411}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B2C9D632-6E8E-4E4D-B849-13347E0E2396}">
@@ -51,6 +59,70 @@
     id=52953c18-2f3e-41e4-9b64-e4b39a6f4685</t>
       </text>
     </comment>
+    <comment ref="A2" authorId="1" shapeId="0" xr:uid="{A496038F-2B69-4D66-8B22-6FE82F201B1B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The name of the Swate template.</t>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="2" shapeId="0" xr:uid="{4FEB2A0D-0D69-4C74-90F9-B60ACAD3FC0E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The current version of this template in SemVer notation.</t>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="3" shapeId="0" xr:uid="{B81587F8-24F1-4441-B5CF-797CFF5344EB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The description of this template. Use few sentences for succinctness.</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="4" shapeId="0" xr:uid="{AB998CBF-C99C-4803-A8E4-15BF70F85D88}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="5" shapeId="0" xr:uid="{702BED30-27FB-4E09-A198-242406CDD04B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The name of the Swate annotation table in the workbook of the template's excel file.</t>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="6" shapeId="0" xr:uid="{6883E21B-C50F-46D5-8D5C-2A49F4678F53}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="7" shapeId="0" xr:uid="{A49430D7-EB67-44F6-A021-4724976004EE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="8" shapeId="0" xr:uid="{E3637547-CF61-40AD-92E9-13EEE0777411}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The author(s) of this template.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -136,9 +208,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Docslink</t>
-  </si>
-  <si>
     <t>Organisation</t>
   </si>
   <si>
@@ -196,18 +265,6 @@
     <t>Authors Affiliation</t>
   </si>
   <si>
-    <t>#AUTHORS ROLES list</t>
-  </si>
-  <si>
-    <t>Authors Roles</t>
-  </si>
-  <si>
-    <t>Authors Roles Term Accession Number</t>
-  </si>
-  <si>
-    <t>Authors Roles Term Source REF</t>
-  </si>
-  <si>
     <t>52953c18-2f3e-41e4-9b64-e4b39a6f4685</t>
   </si>
   <si>
@@ -407,6 +464,21 @@
   </si>
   <si>
     <t>1.1.6</t>
+  </si>
+  <si>
+    <t>Authors Role</t>
+  </si>
+  <si>
+    <t>Authors Role Term Accession Number</t>
+  </si>
+  <si>
+    <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>Authors ORCID</t>
+  </si>
+  <si>
+    <t>DataPLANT</t>
   </si>
 </sst>
 </file>
@@ -417,7 +489,7 @@
     <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,6 +511,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -684,6 +762,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Oliver Maus" id="{CD9B9190-AE51-4CE9-8E50-90F32D97C7F5}" userId="Oliver Maus" providerId="None"/>
+  <person displayName="Kevin F" id="{A2885032-D622-40EE-B371-2F3EF43D5C39}" userId="b000b0ea35d13fa4" providerId="Windows Live"/>
 </personList>
 </file>
 
@@ -987,6 +1066,30 @@
   <threadedComment ref="A1" dT="2021-11-03T16:42:37.57" personId="{CD9B9190-AE51-4CE9-8E50-90F32D97C7F5}" id="{4B404D90-CE94-46B4-87EF-69FB52AFB455}" parentId="{B2C9D632-6E8E-4E4D-B849-13347E0E2396}">
     <text>id=52953c18-2f3e-41e4-9b64-e4b39a6f4685</text>
   </threadedComment>
+  <threadedComment ref="A2" dT="2022-03-04T14:02:18.75" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{A496038F-2B69-4D66-8B22-6FE82F201B1B}">
+    <text>The name of the Swate template.</text>
+  </threadedComment>
+  <threadedComment ref="A3" dT="2022-03-04T14:02:18.76" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{4FEB2A0D-0D69-4C74-90F9-B60ACAD3FC0E}">
+    <text>The current version of this template in SemVer notation.</text>
+  </threadedComment>
+  <threadedComment ref="A4" dT="2022-03-04T14:02:18.76" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{B81587F8-24F1-4441-B5CF-797CFF5344EB}">
+    <text>The description of this template. Use few sentences for succinctness.</text>
+  </threadedComment>
+  <threadedComment ref="A5" dT="2022-03-04T14:02:18.76" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{AB998CBF-C99C-4803-A8E4-15BF70F85D88}">
+    <text>The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2022-03-04T14:02:18.76" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{702BED30-27FB-4E09-A198-242406CDD04B}">
+    <text>The name of the Swate annotation table in the workbook of the template's excel file.</text>
+  </threadedComment>
+  <threadedComment ref="A7" dT="2022-03-04T14:02:18.76" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{6883E21B-C50F-46D5-8D5C-2A49F4678F53}">
+    <text>A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</text>
+  </threadedComment>
+  <threadedComment ref="A11" dT="2022-03-04T14:02:18.77" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{A49430D7-EB67-44F6-A021-4724976004EE}">
+    <text>A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</text>
+  </threadedComment>
+  <threadedComment ref="A15" dT="2022-03-04T14:02:18.77" personId="{A2885032-D622-40EE-B371-2F3EF43D5C39}" id="{E3637547-CF61-40AD-92E9-13EEE0777411}">
+    <text>The author(s) of this template.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1025,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1123,141 +1226,141 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="O2" s="2">
         <v>200</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1267,13 +1370,13 @@
       <c r="N4" s="1"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -1281,23 +1384,23 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1307,13 +1410,13 @@
       <c r="N5" s="1"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -1329,9 +1432,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F787C66-F665-436B-AEA3-3426D484FEC5}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1344,7 +1449,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1352,7 +1457,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1465,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1368,42 +1473,44 @@
         <v>25</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1412,148 +1519,143 @@
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>60</v>
+      <c r="B17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="8"/>
-      <c r="C21" s="10"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="9"/>
+      <c r="A25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
+        <v>113</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="10"/>
+      <c r="A27" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1585,40 +1687,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1626,13 +1728,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -1642,7 +1744,7 @@
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
       <c r="L2" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1650,13 +1752,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
@@ -1666,7 +1768,7 @@
       <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1674,33 +1776,33 @@
         <v>2</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1708,35 +1810,35 @@
         <v>5</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1744,33 +1846,33 @@
         <v>9</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>76</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1778,33 +1880,33 @@
         <v>12</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1812,35 +1914,35 @@
         <v>15</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>94</v>
-      </c>
       <c r="H8" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1848,33 +1950,33 @@
         <v>19</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>